<commit_message>
added all shine bestiaries
</commit_message>
<xml_diff>
--- a/Scripts/python/BestiaryShine.xlsx
+++ b/Scripts/python/BestiaryShine.xlsx
@@ -1089,535 +1089,535 @@
     <t>Блеск · Эвандер Селин</t>
   </si>
   <si>
-    <t>Бестиарий с духом класса C Блеск • Снеголис. Позволяет активировать духа Снеголис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Безмолвная птица. Позволяет активировать духа Безмолвная птица в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Огнемотылек. Позволяет активировать духа Огнемотылек в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Феникс огня. Позволяет активировать духа Феникс огня в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Акула-миньон. Позволяет активировать духа Акула-миньон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Айке. Позволяет активировать духа Айке в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Крут. Позволяет активировать духа Крут в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Пешеход. Позволяет активировать духа Пешеход в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Лиэн. Позволяет активировать духа Лиэн в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Дженсен. Позволяет активировать духа Дженсен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Каллум. Позволяет активировать духа Каллум в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Зефир. Позволяет активировать духа Зефир в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Орландо. Позволяет активировать духа Орландо в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-друид. Позволяет активировать духа Мастер-друид в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-маг. Позволяет активировать духа Мастер-маг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-лучник. Позволяет активировать духа Мастер-лучник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-оборотень. Позволяет активировать духа Мастер-оборотень в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Эйфория. Позволяет активировать духа Эйфория в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Айвен. Позволяет активировать духа Айвен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Камнезов. Позволяет активировать духа Камнезов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Лунная фея. Позволяет активировать духа Лунная фея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Генерал Львов. Позволяет активировать духа Генерал Львов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Главный жрец Фрост. Позволяет активировать духа Главный жрец Фрост в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лорд сумерек. Позволяет активировать духа Лорд сумерек в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I. Блеск Лорда сумерек нельзя разобрать на части.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Зури. Позволяет активировать духа Зури в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Маккени. Позволяет активировать духа Маккени в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Жнец. Позволяет активировать духа Жнец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Дракон мороза. Позволяет активировать духа Дракон мороза в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Сот. Позволяет активировать духа Сот в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I. Блеск Сота нельзя разобрать на части.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Грайммаут. Позволяет активировать духа Грайммаут в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Гидра. Позволяет активировать духа Гидра в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Создатель. Позволяет активировать духа Создатель в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Гаруда. Позволяет активировать духа Гаруда в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Император. Позволяет активировать духа Император в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-жрец. Позволяет активировать духа Мастер-жрец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Мастер-воин. Позволяет активировать духа Мастер-воин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Мастер теней. Позволяет активировать духа Мастер теней в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Фиолетовый тапир. Позволяет активировать духа Фиолетовый тапир в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Жеребец ада. Позволяет активировать духа Жеребец ада в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Буря. Позволяет активировать духа Буря в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Конгамато. Позволяет активировать духа Конгамато в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Царь Чистилища. Позволяет активировать духа Царь Чистилища в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Гонец луны. Позволяет активировать духа Гонец луны в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лорд ада. Позволяет активировать духа Лорд ада в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Владыка лавы. Позволяет активировать духа Владыка лавы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Ноэлл. Позволяет активировать духа Ноэлл в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Брахма. Позволяет активировать духа Брахма в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Морская дева. Позволяет активировать духа Морская дева в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Ведьма. Позволяет активировать духа Ведьма в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Богиня мороза. Позволяет активировать духа Богиня мороза в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Люциан. Позволяет активировать духа Люциан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Нечто. Позволяет активировать духа Нечто в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Черный Роб. Позволяет активировать духа Черный Роб в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Морской демон. Позволяет активировать духа Морской демон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лорд призраков. Позволяет активировать духа Лорд призраков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Мясник. Позволяет активировать духа Мясник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лорд теней. Позволяет активировать духа Лорд теней в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Страж руин. Позволяет активировать духа Страж руин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Бог мечей. Позволяет активировать духа Бог мечей в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Айрин . Позволяет активировать духа Айрин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Голова паразита. Позволяет активировать духа Голова паразита в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Шоу Лу. Позволяет активировать духа Шоу Лу в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Генерал Цинь. Позволяет активировать духа Генерал Цинь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Финиас. Позволяет активировать духа Финиас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Дитя демона. Позволяет активировать духа Дитя демона в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Ведьма Цзян Гу. Позволяет активировать духа Ведьма Цзян Гу в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лицемер. Позволяет активировать духа Лицемер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Линус. Позволяет активировать духа Линус в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Властелин тьмы. Позволяет активировать духа Властелин тьмы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Гибрид. Позволяет активировать духа Гибрид в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Эмиссар. Позволяет активировать духа Эмиссар в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Душегуб. Позволяет активировать духа Душегуб в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Инсект. Позволяет активировать духа Инсект в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Харон. Позволяет активировать духа Харон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Древо жизни. Позволяет активировать духа Древо жизни в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Барон. Позволяет активировать духа Барон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Король суховеев. Позволяет активировать духа Король суховеев в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Чэнь Минцзэ. Позволяет активировать духа Чэнь Минцзэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Дознаватель. Позволяет активировать духа Дознаватель в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Око пустоты. Позволяет активировать духа Око пустоты в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Маска. Позволяет активировать духа Маска в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Падший бог. Позволяет активировать духа Падший бог в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Сёгун. Позволяет активировать духа Сёгун в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I. Блеск Сёгуна нельзя разобрать на части.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хармони. Позволяет активировать духа Хармони в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Тинто. Позволяет активировать духа Тинто в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Юнона. Позволяет активировать духа Юнона в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лиша. Позволяет активировать духа Лиша в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Космофаг. Позволяет активировать духа Космофаг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I. Блеск Космофага нельзя разобрать на части.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Ворожея. Позволяет активировать духа Ворожея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Сатх. Позволяет активировать духа Сатх в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Мудрый Сатх. Позволяет активировать духа Мудрый Сатх в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Профессор Сон. Позволяет активировать духа Профессор Сон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Королева-людоед. Позволяет активировать духа Королева-людоед в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Башня чар. Позволяет активировать духа Башня чар в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Янци. Позволяет активировать духа Янци в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Лин. Позволяет активировать духа Лин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Старейшина Лис. Позволяет активировать духа Старейшина Лис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Ст. Снежный лис. Позволяет активировать духа Ст. Снежный лис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Громовой лич. Позволяет активировать духа Громовой лич в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Проклятый ужас. Позволяет активировать духа Проклятый ужас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Лорд Быков. Позволяет активировать духа Лорд Быков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Лорд Волков. Позволяет активировать духа Лорд Волков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Лорд Крыс. Позволяет активировать духа Лорд Крыс в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Лорд Львов. Позволяет активировать духа Лорд Львов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Эвандер / Селин. Позволяет активировать духа Эвандер / Селин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Безголовый рыцарь. Позволяет активировать духа Безголовый рыцарь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Старейшина Элизиума. Позволяет активировать духа Старейшина Элизиума в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Волк-посланец. Позволяет активировать духа Волк-посланец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Святой посланец. Позволяет активировать духа Святой посланец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Джексон. Позволяет активировать духа Джексон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса B Блеск • Риан. Позволяет активировать духа Риан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Белка-летяга. Позволяет активировать духа Белка-летяга в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Летучая лиса. Позволяет активировать духа Летучая лиса в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Бессмертный демон. Позволяет активировать духа Бессмертный демон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Небесный ящер. Позволяет активировать духа Небесный ящер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса C Блеск • Флибустьер. Позволяет активировать духа Флибустьер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Сати. Позволяет активировать духа Сати в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Сатори. Позволяет активировать духа Сатори в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Божество. Позволяет активировать духа Божество в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Рассвет. Позволяет активировать духа Рассвет в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • День. Позволяет активировать духа День в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Чхуан. Позволяет активировать духа Чхуан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хиэм. Позволяет активировать духа Хиэм в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Люмен. Позволяет активировать духа Люмен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Обсидиан. Позволяет активировать духа Обсидиан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса А Блеск • Темный странник. Позволяет активировать духа Темный странник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Память. Позволяет активировать духа Память в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Будущее. Позволяет активировать духа Будущее в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Синдикат. Позволяет активировать духа Синдикат в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Глубокое море. Позволяет активировать духа Глубокое море в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Воля Чию. Позволяет активировать духа Воля Чию в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лин Яо. Позволяет активировать духа Лин Яо в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Цай И. Позволяет активировать духа Цай И в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Страж горы. Позволяет активировать духа Страж горы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Бог Джа. Позволяет активировать духа Бог Джа в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Вэй И. Позволяет активировать духа Вэй И в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хуай Сюэ. Позволяет активировать духа Хуай Сюэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Ша. Позволяет активировать духа Ша в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Маммон. Позволяет активировать духа Маммон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Пятый принц. Позволяет активировать духа Пятый принц в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Жан. Позволяет активировать духа Жан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Дракос. Позволяет активировать духа Дракос в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Вуй Юэ. Позволяет активировать духа Вуй Юэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хэ Юньян. Позволяет активировать духа Хэ Юньян в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Инь Хуан. Позволяет активировать духа Инь Хуан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Цан Лань. Позволяет активировать духа Цан Лань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Айя. Позволяет активировать духа Айя в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Искуситель. Позволяет активировать духа Искуситель в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Невежда. Позволяет активировать духа Невежда в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Владыка ада. Позволяет активировать духа Владыка ада в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Кродха. Позволяет активировать духа Кродха в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S [Блеск] Си Сюань. Позволяет активировать духа Си Сюань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S [Блеск] Кира. Позволяет активировать духа Кира в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S [Блеск] Эзра. Позволяет активировать духа Эзра в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S [Блеск] Астрас. Позволяет активировать духа Астрас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A [Блеск] Лу Юйчжэнь. Позволяет активировать духа Лу Юйчжэнь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хун Чию · Пламя. Позволяет активировать духа Хун Чию · Пламя в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Рури · Путь. Позволяет активировать духа Рури · Путь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Князь ашуров. Позволяет активировать духа Князь ашуров в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Лу Юйбай. Позволяет активировать духа Лу Юйбай в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Чжу Юнь. Позволяет активировать духа Чжу Юнь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>22_159506_Бестиарий с духом класса S Блеск • 燕于归. Позволяет активировать духа 燕于归 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Чэн Инянь. Позволяет активировать духа Чэн Инянь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>22_159546_Бестиарий с духом класса S Блеск • 凤凰·真神. Позволяет активировать духа 凤凰·真神 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Барс Янг. Позволяет активировать духа Барс Янг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>22_159586_Бестиарий с духом класса A Блеск • 宁宵. Позволяет активировать духа 宁宵 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Аргус. Позволяет активировать духа Аргус в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска уже активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I.</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Абрис. Позволяет активировать духа Абрис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Царь драконов. Позволяет активировать духа Царь драконов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Кира · Наяда. Позволяет активировать духа Кира · Наяда в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Эзра · Змея. Позволяет активировать духа Эзра · Змея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Астрас · Дракон. Позволяет активировать духа Астрас · Дракон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Хун Чию. Позволяет активировать духа Хун Чию в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Рури. Позволяет активировать духа Рури в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Чун-Хуа. Позволяет активировать духа Чун-Хуа в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса S Блеск • Цзюнь Мао. Позволяет активировать духа Цзюнь Мао в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с Пламенем начала I</t>
-  </si>
-  <si>
-    <t>Бестиарий с духом класса A Блеск • Нин'ань. Позволяет активировать духа Нин'ань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с Пламенем начала I</t>
+    <t>Бестиарий с духом класса S [Блеск] Си Сюань. Позволяет активировать духа Си Сюань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S [Блеск] Кира. Позволяет активировать духа Кира в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S [Блеск] Эзра. Позволяет активировать духа Эзра в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S [Блеск] Астрас. Позволяет активировать духа Астрас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A [Блеск] Лу Юйчжэнь. Позволяет активировать духа Лу Юйчжэнь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Безмолвная птица. Позволяет активировать духа Безмолвная птица в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Огнемотылек. Позволяет активировать духа Огнемотылек в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Феникс огня. Позволяет активировать духа Феникс огня в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Акула-миньон. Позволяет активировать духа Акула-миньон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Айке. Позволяет активировать духа Айке в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Крут. Позволяет активировать духа Крут в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Пешеход. Позволяет активировать духа Пешеход в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Лиэн. Позволяет активировать духа Лиэн в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Дженсен. Позволяет активировать духа Дженсен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Каллум. Позволяет активировать духа Каллум в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Зефир. Позволяет активировать духа Зефир в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Орландо. Позволяет активировать духа Орландо в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-друид. Позволяет активировать духа Мастер-друид в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-маг. Позволяет активировать духа Мастер-маг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-лучник. Позволяет активировать духа Мастер-лучник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-оборотень. Позволяет активировать духа Мастер-оборотень в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Эйфория. Позволяет активировать духа Эйфория в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Айвен. Позволяет активировать духа Айвен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Камнезов. Позволяет активировать духа Камнезов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Лунная фея. Позволяет активировать духа Лунная фея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Генерал Львов. Позволяет активировать духа Генерал Львов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Главный жрец Фрост. Позволяет активировать духа Главный жрец Фрост в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лорд сумерек. Позволяет активировать духа Лорд сумерек в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]. Блеск Лорда сумерек нельзя разобрать на части.</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Зури. Позволяет активировать духа Зури в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Маккени. Позволяет активировать духа Маккени в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Жнец. Позволяет активировать духа Жнец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Дракон мороза. Позволяет активировать духа Дракон мороза в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Сот. Позволяет активировать духа Сот в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]. Блеск Сота нельзя разобрать на части.</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Грайммаут. Позволяет активировать духа Грайммаут в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Гидра. Позволяет активировать духа Гидра в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Создатель. Позволяет активировать духа Создатель в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Гаруда. Позволяет активировать духа Гаруда в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Император. Позволяет активировать духа Император в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-жрец. Позволяет активировать духа Мастер-жрец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Мастер-воин. Позволяет активировать духа Мастер-воин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Мастер теней. Позволяет активировать духа Мастер теней в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Фиолетовый тапир. Позволяет активировать духа Фиолетовый тапир в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Жеребец ада. Позволяет активировать духа Жеребец ада в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Буря. Позволяет активировать духа Буря в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Конгамато. Позволяет активировать духа Конгамато в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Царь Чистилища. Позволяет активировать духа Царь Чистилища в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Гонец луны. Позволяет активировать духа Гонец луны в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лорд ада. Позволяет активировать духа Лорд ада в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Владыка лавы. Позволяет активировать духа Владыка лавы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Ноэлл. Позволяет активировать духа Ноэлл в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Брахма. Позволяет активировать духа Брахма в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Морская дева. Позволяет активировать духа Морская дева в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Ведьма. Позволяет активировать духа Ведьма в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Богиня мороза. Позволяет активировать духа Богиня мороза в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Люциан. Позволяет активировать духа Люциан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Нечто. Позволяет активировать духа Нечто в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Черный Роб. Позволяет активировать духа Черный Роб в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Морской демон. Позволяет активировать духа Морской демон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лорд призраков. Позволяет активировать духа Лорд призраков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Мясник. Позволяет активировать духа Мясник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лорд теней. Позволяет активировать духа Лорд теней в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Страж руин. Позволяет активировать духа Страж руин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Бог мечей. Позволяет активировать духа Бог мечей в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Айрин . Позволяет активировать духа Айрин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Голова паразита. Позволяет активировать духа Голова паразита в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Шоу Лу. Позволяет активировать духа Шоу Лу в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Генерал Цинь. Позволяет активировать духа Генерал Цинь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Финиас. Позволяет активировать духа Финиас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Дитя демона. Позволяет активировать духа Дитя демона в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Ведьма Цзян Гу. Позволяет активировать духа Ведьма Цзян Гу в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лицемер. Позволяет активировать духа Лицемер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Линус. Позволяет активировать духа Линус в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Властелин тьмы. Позволяет активировать духа Властелин тьмы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Гибрид. Позволяет активировать духа Гибрид в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Эмиссар. Позволяет активировать духа Эмиссар в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Душегуб. Позволяет активировать духа Душегуб в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Инсект. Позволяет активировать духа Инсект в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Харон. Позволяет активировать духа Харон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Древо жизни. Позволяет активировать духа Древо жизни в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Барон. Позволяет активировать духа Барон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Король суховеев. Позволяет активировать духа Король суховеев в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Чэнь Минцзэ. Позволяет активировать духа Чэнь Минцзэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Дознаватель. Позволяет активировать духа Дознаватель в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Око пустоты. Позволяет активировать духа Око пустоты в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Маска. Позволяет активировать духа Маска в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Падший бог. Позволяет активировать духа Падший бог в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Сёгун. Позволяет активировать духа Сёгун в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]. Блеск Сёгуна нельзя разобрать на части.</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хармони. Позволяет активировать духа Хармони в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Тинто. Позволяет активировать духа Тинто в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Юнона. Позволяет активировать духа Юнона в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лиша. Позволяет активировать духа Лиша в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Космофаг. Позволяет активировать духа Космофаг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]. Блеск Космофага нельзя разобрать на части.</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Аргус. Позволяет активировать духа Аргус в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска уже активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Ворожея. Позволяет активировать духа Ворожея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Сатх. Позволяет активировать духа Сатх в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Мудрый Сатх. Позволяет активировать духа Мудрый Сатх в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Профессор Сон. Позволяет активировать духа Профессор Сон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Королева-людоед. Позволяет активировать духа Королева-людоед в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Башня чар. Позволяет активировать духа Башня чар в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Янци. Позволяет активировать духа Янци в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Лин. Позволяет активировать духа Лин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Старейшина Лис. Позволяет активировать духа Старейшина Лис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Ст. Снежный лис. Позволяет активировать духа Ст. Снежный лис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Громовой лич. Позволяет активировать духа Громовой лич в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Проклятый ужас. Позволяет активировать духа Проклятый ужас в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Лорд Быков. Позволяет активировать духа Лорд Быков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Лорд Волков. Позволяет активировать духа Лорд Волков в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Лорд Крыс. Позволяет активировать духа Лорд Крыс в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Лорд Львов. Позволяет активировать духа Лорд Львов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Эвандер / Селин. Позволяет активировать духа Эвандер / Селин в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Безголовый рыцарь. Позволяет активировать духа Безголовый рыцарь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Старейшина Элизиума. Позволяет активировать духа Старейшина Элизиума в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Волк-посланец. Позволяет активировать духа Волк-посланец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Святой посланец. Позволяет активировать духа Святой посланец в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Джексон. Позволяет активировать духа Джексон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса B Блеск · Риан. Позволяет активировать духа Риан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Белка-летяга. Позволяет активировать духа Белка-летяга в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Летучая лиса. Позволяет активировать духа Летучая лиса в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Бессмертный демон. Позволяет активировать духа Бессмертный демон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Небесный ящер. Позволяет активировать духа Небесный ящер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C Блеск · Флибустьер. Позволяет активировать духа Флибустьер в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Сати. Позволяет активировать духа Сати в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Сатори. Позволяет активировать духа Сатори в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Божество. Позволяет активировать духа Божество в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Рассвет. Позволяет активировать духа Рассвет в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · День. Позволяет активировать духа День в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Чхуан. Позволяет активировать духа Чхуан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хиэм. Позволяет активировать духа Хиэм в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Люмен. Позволяет активировать духа Люмен в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Обсидиан. Позволяет активировать духа Обсидиан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса А Блеск · Темный странник. Позволяет активировать духа Темный странник в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Память. Позволяет активировать духа Память в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Будущее. Позволяет активировать духа Будущее в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Синдикат. Позволяет активировать духа Синдикат в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Глубокое море. Позволяет активировать духа Глубокое море в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Воля Чию. Позволяет активировать духа Воля Чию в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лин Яо. Позволяет активировать духа Лин Яо в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Цай И. Позволяет активировать духа Цай И в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Страж горы. Позволяет активировать духа Страж горы в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Бог Джа. Позволяет активировать духа Бог Джа в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Вэй И. Позволяет активировать духа Вэй И в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хуай Сюэ. Позволяет активировать духа Хуай Сюэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Ша. Позволяет активировать духа Ша в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Маммон. Позволяет активировать духа Маммон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Пятый принц. Позволяет активировать духа Пятый принц в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Жан. Позволяет активировать духа Жан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Дракос. Позволяет активировать духа Дракос в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Вуй Юэ. Позволяет активировать духа Вуй Юэ в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хэ Юньян. Позволяет активировать духа Хэ Юньян в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Инь Хуан. Позволяет активировать духа Инь Хуан в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Цан Лань. Позволяет активировать духа Цан Лань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Айя. Позволяет активировать духа Айя в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Искуситель. Позволяет активировать духа Искуситель в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Невежда. Позволяет активировать духа Невежда в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Владыка ада. Позволяет активировать духа Владыка ада в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Кродха. Позволяет активировать духа Кродха в режиме сияния. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим сияния этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Абрис. Позволяет активировать духа Абрис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Царь драконов. Позволяет активировать духа Царь драконов в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Кира · Наяда. Позволяет активировать духа Кира · Наяда в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Эзра · Змея. Позволяет активировать духа Эзра · Змея в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Астрас · Дракон. Позволяет активировать духа Астрас · Дракон в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хун Чию. Позволяет активировать духа Хун Чию в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Рури. Позволяет активировать духа Рури в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Чун-Хуа. Позволяет активировать духа Чун-Хуа в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Цзюнь Мао. Позволяет активировать духа Цзюнь Мао в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Нин'ань. Позволяет активировать духа Нин'ань в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]]</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Хун Чию · Пламя. Позволяет активировать духа Хун Чию · Пламя в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Рури · Путь. Позволяет активировать духа Рури · Путь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Князь ашуров. Позволяет активировать духа Князь ашуров в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Лу Юйбай. Позволяет активировать духа Лу Юйбай в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса A Блеск · Чжу Юнь. Позволяет активировать духа Чжу Юнь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>22_159506_Бестиарий с духом класса S Блеск · 燕于归. Позволяет активировать духа 燕于归 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Чэн Инянь. Позволяет активировать духа Чэн Инянь в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>22_159546_Бестиарий с духом класса S Блеск · 凤凰·真神. Позволяет активировать духа 凤凰·真神 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса S Блеск · Барс Янг. Позволяет активировать духа Барс Янг в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна. Можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>22_159586_Бестиарий с духом класса A Блеск · 宁宵. Позволяет активировать духа 宁宵 в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
+  </si>
+  <si>
+    <t>Бестиарий с духом класса C [[Блеск · Снеголис]]. Позволяет активировать духа Снеголис в режиме Блеска. Активация повышает статы духа на 15%. Активировать режим можно только после призыва духа. Если режим Блеска этого духа уже был активирован, повторная активация невозможна, можно переплавить в пыль духа в горне с [[Пламя начала I]].</t>
   </si>
 </sst>
 </file>
@@ -2061,7 +2061,7 @@
   <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,14 +2085,14 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2100,18 +2100,18 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>358</v>
+      <c r="C4" s="4" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="132" x14ac:dyDescent="0.25">
@@ -2122,10 +2122,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2133,10 +2133,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2144,10 +2144,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2155,10 +2155,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -2166,10 +2166,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2177,10 +2177,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2188,10 +2188,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2199,10 +2199,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2210,10 +2210,10 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -2221,10 +2221,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -2232,10 +2232,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -2243,10 +2243,10 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2254,10 +2254,10 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -2265,10 +2265,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -2276,10 +2276,10 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -2287,10 +2287,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -2298,10 +2298,10 @@
         <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -2309,10 +2309,10 @@
         <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
@@ -2320,10 +2320,10 @@
         <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
@@ -2342,10 +2342,10 @@
         <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="132" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -2353,10 +2353,10 @@
         <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2364,10 +2364,10 @@
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2375,10 +2375,10 @@
         <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -2386,10 +2386,10 @@
         <v>58</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
@@ -2397,10 +2397,10 @@
         <v>60</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -2408,10 +2408,10 @@
         <v>62</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -2419,10 +2419,10 @@
         <v>64</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -2430,10 +2430,10 @@
         <v>66</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -2441,10 +2441,10 @@
         <v>68</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>69</v>
       </c>
@@ -2452,10 +2452,10 @@
         <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -2463,10 +2463,10 @@
         <v>72</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>73</v>
       </c>
@@ -2474,10 +2474,10 @@
         <v>74</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>75</v>
       </c>
@@ -2485,10 +2485,10 @@
         <v>76</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>77</v>
       </c>
@@ -2496,10 +2496,10 @@
         <v>78</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>79</v>
       </c>
@@ -2507,10 +2507,10 @@
         <v>80</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
@@ -2518,10 +2518,10 @@
         <v>82</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>83</v>
       </c>
@@ -2529,10 +2529,10 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>85</v>
       </c>
@@ -2540,10 +2540,10 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -2551,10 +2551,10 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>89</v>
       </c>
@@ -2562,10 +2562,10 @@
         <v>90</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>91</v>
       </c>
@@ -2573,10 +2573,10 @@
         <v>92</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
@@ -2584,10 +2584,10 @@
         <v>94</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>95</v>
       </c>
@@ -2595,10 +2595,10 @@
         <v>96</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
@@ -2606,10 +2606,10 @@
         <v>98</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
@@ -2617,10 +2617,10 @@
         <v>100</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>101</v>
       </c>
@@ -2628,10 +2628,10 @@
         <v>102</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>103</v>
       </c>
@@ -2639,10 +2639,10 @@
         <v>104</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -2650,10 +2650,10 @@
         <v>106</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>107</v>
       </c>
@@ -2661,10 +2661,10 @@
         <v>108</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>109</v>
       </c>
@@ -2672,10 +2672,10 @@
         <v>110</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -2683,10 +2683,10 @@
         <v>112</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>113</v>
       </c>
@@ -2694,10 +2694,10 @@
         <v>114</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>115</v>
       </c>
@@ -2705,10 +2705,10 @@
         <v>116</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>117</v>
       </c>
@@ -2716,10 +2716,10 @@
         <v>118</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>119</v>
       </c>
@@ -2727,10 +2727,10 @@
         <v>120</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>121</v>
       </c>
@@ -2738,10 +2738,10 @@
         <v>122</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>123</v>
       </c>
@@ -2749,10 +2749,10 @@
         <v>124</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -2760,10 +2760,10 @@
         <v>126</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>127</v>
       </c>
@@ -2771,10 +2771,10 @@
         <v>128</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>129</v>
       </c>
@@ -2782,10 +2782,10 @@
         <v>130</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>131</v>
       </c>
@@ -2793,10 +2793,10 @@
         <v>132</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>133</v>
       </c>
@@ -2804,10 +2804,10 @@
         <v>134</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>135</v>
       </c>
@@ -2815,10 +2815,10 @@
         <v>136</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>137</v>
       </c>
@@ -2826,10 +2826,10 @@
         <v>138</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>139</v>
       </c>
@@ -2837,10 +2837,10 @@
         <v>140</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>141</v>
       </c>
@@ -2848,10 +2848,10 @@
         <v>142</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
@@ -2859,10 +2859,10 @@
         <v>144</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>145</v>
       </c>
@@ -2870,10 +2870,10 @@
         <v>146</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>147</v>
       </c>
@@ -2881,10 +2881,10 @@
         <v>148</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>149</v>
       </c>
@@ -2892,10 +2892,10 @@
         <v>150</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>151</v>
       </c>
@@ -2903,10 +2903,10 @@
         <v>152</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>153</v>
       </c>
@@ -2914,10 +2914,10 @@
         <v>154</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>155</v>
       </c>
@@ -2925,10 +2925,10 @@
         <v>156</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>157</v>
       </c>
@@ -2936,10 +2936,10 @@
         <v>158</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>159</v>
       </c>
@@ -2947,10 +2947,10 @@
         <v>160</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>161</v>
       </c>
@@ -2958,10 +2958,10 @@
         <v>162</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>163</v>
       </c>
@@ -2969,10 +2969,10 @@
         <v>164</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>165</v>
       </c>
@@ -2980,10 +2980,10 @@
         <v>166</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>167</v>
       </c>
@@ -2991,10 +2991,10 @@
         <v>168</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>169</v>
       </c>
@@ -3002,10 +3002,10 @@
         <v>170</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>171</v>
       </c>
@@ -3013,10 +3013,10 @@
         <v>172</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>173</v>
       </c>
@@ -3024,10 +3024,10 @@
         <v>174</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>175</v>
       </c>
@@ -3035,10 +3035,10 @@
         <v>176</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>177</v>
       </c>
@@ -3046,10 +3046,10 @@
         <v>178</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>179</v>
       </c>
@@ -3057,10 +3057,10 @@
         <v>180</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>181</v>
       </c>
@@ -3068,10 +3068,10 @@
         <v>182</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>183</v>
       </c>
@@ -3079,10 +3079,10 @@
         <v>184</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>185</v>
       </c>
@@ -3090,10 +3090,10 @@
         <v>186</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>187</v>
       </c>
@@ -3101,10 +3101,10 @@
         <v>188</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>189</v>
       </c>
@@ -3112,10 +3112,10 @@
         <v>190</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>191</v>
       </c>
@@ -3123,10 +3123,10 @@
         <v>192</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>193</v>
       </c>
@@ -3134,10 +3134,10 @@
         <v>194</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>195</v>
       </c>
@@ -3145,10 +3145,10 @@
         <v>196</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>197</v>
       </c>
@@ -3156,10 +3156,10 @@
         <v>198</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>199</v>
       </c>
@@ -3167,10 +3167,10 @@
         <v>200</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>201</v>
       </c>
@@ -3178,10 +3178,10 @@
         <v>202</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>203</v>
       </c>
@@ -3189,10 +3189,10 @@
         <v>204</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>205</v>
       </c>
@@ -3200,10 +3200,10 @@
         <v>206</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>207</v>
       </c>
@@ -3211,10 +3211,10 @@
         <v>208</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>209</v>
       </c>
@@ -3222,10 +3222,10 @@
         <v>210</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>211</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>212</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="132" x14ac:dyDescent="0.25">
@@ -3244,10 +3244,10 @@
         <v>355</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>214</v>
       </c>
@@ -3255,10 +3255,10 @@
         <v>215</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>216</v>
       </c>
@@ -3266,10 +3266,10 @@
         <v>217</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>218</v>
       </c>
@@ -3277,10 +3277,10 @@
         <v>219</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>220</v>
       </c>
@@ -3288,10 +3288,10 @@
         <v>221</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>222</v>
       </c>
@@ -3299,10 +3299,10 @@
         <v>223</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>224</v>
       </c>
@@ -3310,10 +3310,10 @@
         <v>225</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>226</v>
       </c>
@@ -3321,10 +3321,10 @@
         <v>227</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>228</v>
       </c>
@@ -3332,10 +3332,10 @@
         <v>229</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>230</v>
       </c>
@@ -3343,10 +3343,10 @@
         <v>231</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>232</v>
       </c>
@@ -3354,10 +3354,10 @@
         <v>233</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>234</v>
       </c>
@@ -3365,10 +3365,10 @@
         <v>235</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>236</v>
       </c>
@@ -3376,10 +3376,10 @@
         <v>237</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>238</v>
       </c>
@@ -3387,10 +3387,10 @@
         <v>239</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>240</v>
       </c>
@@ -3398,10 +3398,10 @@
         <v>241</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>242</v>
       </c>
@@ -3409,10 +3409,10 @@
         <v>243</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>244</v>
       </c>
@@ -3420,10 +3420,10 @@
         <v>245</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>246</v>
       </c>
@@ -3431,10 +3431,10 @@
         <v>247</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>248</v>
       </c>
@@ -3442,10 +3442,10 @@
         <v>249</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>250</v>
       </c>
@@ -3453,10 +3453,10 @@
         <v>251</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>252</v>
       </c>
@@ -3464,10 +3464,10 @@
         <v>253</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>254</v>
       </c>
@@ -3475,10 +3475,10 @@
         <v>255</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>256</v>
       </c>
@@ -3486,10 +3486,10 @@
         <v>257</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>258</v>
       </c>
@@ -3497,10 +3497,10 @@
         <v>259</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>260</v>
       </c>
@@ -3508,10 +3508,10 @@
         <v>261</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>262</v>
       </c>
@@ -3519,10 +3519,10 @@
         <v>263</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>264</v>
       </c>
@@ -3530,10 +3530,10 @@
         <v>265</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>266</v>
       </c>
@@ -3541,10 +3541,10 @@
         <v>267</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>268</v>
       </c>
@@ -3552,10 +3552,10 @@
         <v>269</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>270</v>
       </c>
@@ -3563,10 +3563,10 @@
         <v>271</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>272</v>
       </c>
@@ -3574,10 +3574,10 @@
         <v>273</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>274</v>
       </c>
@@ -3585,10 +3585,10 @@
         <v>275</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>276</v>
       </c>
@@ -3596,10 +3596,10 @@
         <v>277</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>278</v>
       </c>
@@ -3607,10 +3607,10 @@
         <v>279</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>280</v>
       </c>
@@ -3618,10 +3618,10 @@
         <v>281</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>282</v>
       </c>
@@ -3629,10 +3629,10 @@
         <v>283</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>284</v>
       </c>
@@ -3640,10 +3640,10 @@
         <v>285</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>286</v>
       </c>
@@ -3651,10 +3651,10 @@
         <v>287</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>288</v>
       </c>
@@ -3662,10 +3662,10 @@
         <v>289</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>290</v>
       </c>
@@ -3673,10 +3673,10 @@
         <v>291</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>292</v>
       </c>
@@ -3684,10 +3684,10 @@
         <v>293</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>294</v>
       </c>
@@ -3695,10 +3695,10 @@
         <v>295</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>296</v>
       </c>
@@ -3706,10 +3706,10 @@
         <v>297</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>298</v>
       </c>
@@ -3717,10 +3717,10 @@
         <v>299</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>300</v>
       </c>
@@ -3728,10 +3728,10 @@
         <v>301</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>302</v>
       </c>
@@ -3739,10 +3739,10 @@
         <v>303</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>304</v>
       </c>
@@ -3750,10 +3750,10 @@
         <v>305</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>306</v>
       </c>
@@ -3761,10 +3761,10 @@
         <v>307</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>308</v>
       </c>
@@ -3772,10 +3772,10 @@
         <v>309</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>310</v>
       </c>
@@ -3783,10 +3783,10 @@
         <v>311</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>312</v>
       </c>
@@ -3794,10 +3794,10 @@
         <v>313</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>314</v>
       </c>
@@ -3805,10 +3805,10 @@
         <v>315</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>316</v>
       </c>
@@ -3816,10 +3816,10 @@
         <v>317</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>318</v>
       </c>
@@ -3827,10 +3827,10 @@
         <v>319</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>320</v>
       </c>
@@ -3838,10 +3838,10 @@
         <v>321</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>322</v>
       </c>
@@ -3849,10 +3849,10 @@
         <v>323</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>324</v>
       </c>
@@ -3860,10 +3860,10 @@
         <v>325</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>326</v>
       </c>
@@ -3871,10 +3871,10 @@
         <v>327</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>328</v>
       </c>
@@ -3882,10 +3882,10 @@
         <v>329</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>330</v>
       </c>
@@ -3893,10 +3893,10 @@
         <v>331</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>332</v>
       </c>
@@ -3904,10 +3904,10 @@
         <v>333</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>334</v>
       </c>
@@ -3915,10 +3915,10 @@
         <v>335</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>336</v>
       </c>
@@ -3926,10 +3926,10 @@
         <v>327</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>337</v>
       </c>
@@ -3937,10 +3937,10 @@
         <v>338</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>339</v>
       </c>
@@ -3948,10 +3948,10 @@
         <v>340</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>341</v>
       </c>
@@ -3959,10 +3959,10 @@
         <v>342</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>343</v>
       </c>
@@ -3970,10 +3970,10 @@
         <v>344</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>345</v>
       </c>
@@ -3981,10 +3981,10 @@
         <v>346</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>347</v>
       </c>
@@ -3992,10 +3992,10 @@
         <v>348</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>349</v>
       </c>
@@ -4003,10 +4003,10 @@
         <v>350</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>351</v>
       </c>
@@ -4014,10 +4014,10 @@
         <v>352</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="148.5" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>353</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>354</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>